<commit_message>
updated ipsec tunnel ip-ip
</commit_message>
<xml_diff>
--- a/All-in-one/all-variablefile.xlsx
+++ b/All-in-one/all-variablefile.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAAFAT.SOLIMAN\PycharmProjects\All-in-one\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RAAFAT.SOLIMAN\PaloAlto-Scripts\Palo-Alto-Scripts\PaloAlto-Scripts\All-in-one\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A554BB0E-2623-4EA3-B05D-11336CB52BE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3F185C7-05BF-4F4A-B5C8-6366F8C58F4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{9F0FD438-5775-4B9C-9AB4-79BE4477D7DD}"/>
+    <workbookView xWindow="-28920" yWindow="-3990" windowWidth="29040" windowHeight="15720" xr2:uid="{9F0FD438-5775-4B9C-9AB4-79BE4477D7DD}"/>
   </bookViews>
   <sheets>
     <sheet name="variablefile" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="145">
   <si>
     <t>device_ip</t>
   </si>
@@ -37,9 +37,6 @@
     <t>hostname</t>
   </si>
   <si>
-    <t>TESTC16</t>
-  </si>
-  <si>
     <t>interface_ethernet1_1</t>
   </si>
   <si>
@@ -55,27 +52,15 @@
     <t>ethernet1_1_ip</t>
   </si>
   <si>
-    <t>10.34.1.1/28</t>
-  </si>
-  <si>
     <t>ethernet1_2_ip</t>
   </si>
   <si>
-    <t>10.34.152.113/28</t>
-  </si>
-  <si>
     <t>interface_management_profile_ethernet1_1</t>
   </si>
   <si>
-    <t>Ping</t>
-  </si>
-  <si>
     <t>interface_management_profile_ethernet1_2</t>
   </si>
   <si>
-    <t>PING HTTPS SSH</t>
-  </si>
-  <si>
     <t>loopback_interface</t>
   </si>
   <si>
@@ -148,30 +133,6 @@
     <t>dns_interface</t>
   </si>
   <si>
-    <t>dhcp_interface</t>
-  </si>
-  <si>
-    <t>dhcp_ip_pool</t>
-  </si>
-  <si>
-    <t>10.34.152.112/28</t>
-  </si>
-  <si>
-    <t>dhcp_dns_primary</t>
-  </si>
-  <si>
-    <t>10.34.152.113</t>
-  </si>
-  <si>
-    <t>dhcp_gateway</t>
-  </si>
-  <si>
-    <t>10.34.152.114</t>
-  </si>
-  <si>
-    <t>dhcp_subnet_mask</t>
-  </si>
-  <si>
     <t>service_interface</t>
   </si>
   <si>
@@ -181,9 +142,6 @@
     <t>ike_gateway_name</t>
   </si>
   <si>
-    <t>IPSec_Gateway_PHC</t>
-  </si>
-  <si>
     <t>pre_shared_key</t>
   </si>
   <si>
@@ -196,24 +154,12 @@
     <t>peer_address</t>
   </si>
   <si>
-    <t>102.90.33.172</t>
-  </si>
-  <si>
-    <t>ufqdn_local_id</t>
-  </si>
-  <si>
-    <t>jeroen.schellart@shell.com</t>
-  </si>
-  <si>
     <t>peer_id</t>
   </si>
   <si>
     <t>ipsec_tunnel_name</t>
   </si>
   <si>
-    <t>IPSec_Tunnel_PHC</t>
-  </si>
-  <si>
     <t>redist_interface</t>
   </si>
   <si>
@@ -343,9 +289,6 @@
     <t>private_network_interfaces</t>
   </si>
   <si>
-    <t>[ethernet1/2, tunnel.1, loopback.103]</t>
-  </si>
-  <si>
     <t>security_rule_name</t>
   </si>
   <si>
@@ -395,13 +338,130 @@
   </si>
   <si>
     <t>nat_rule_source_zone</t>
+  </si>
+  <si>
+    <t>Raafat-FW</t>
+  </si>
+  <si>
+    <t>10.1.1.1/24</t>
+  </si>
+  <si>
+    <t>PING</t>
+  </si>
+  <si>
+    <t>interface_management_profile_ethernet1_6</t>
+  </si>
+  <si>
+    <t>ethernet1_6_ip</t>
+  </si>
+  <si>
+    <t>interface_ethernet1_6</t>
+  </si>
+  <si>
+    <t>ethernet1/6</t>
+  </si>
+  <si>
+    <t>dhcp_interface_A</t>
+  </si>
+  <si>
+    <t>dhcp_ip_pool_A</t>
+  </si>
+  <si>
+    <t>dhcp_dns_primary_A</t>
+  </si>
+  <si>
+    <t>dhcp_gateway_A</t>
+  </si>
+  <si>
+    <t>dhcp_subnet_mask_A</t>
+  </si>
+  <si>
+    <t>dhcp_interface_B</t>
+  </si>
+  <si>
+    <t>dhcp_ip_pool_B</t>
+  </si>
+  <si>
+    <t>dhcp_dns_primary_B</t>
+  </si>
+  <si>
+    <t>dhcp_gateway_B</t>
+  </si>
+  <si>
+    <t>dhcp_subnet_mask_B</t>
+  </si>
+  <si>
+    <t>10.6.6.0/24</t>
+  </si>
+  <si>
+    <t>10.2.2.1/24</t>
+  </si>
+  <si>
+    <t>10.3.3.1/32</t>
+  </si>
+  <si>
+    <t>10.6.6.1/24</t>
+  </si>
+  <si>
+    <t>10.2.2.1</t>
+  </si>
+  <si>
+    <t>10.6.6.1</t>
+  </si>
+  <si>
+    <t>PING-HTTPS-SSH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ethernet1/2 ethernet1/6 loopback.103 tunnel.1 </t>
+  </si>
+  <si>
+    <t>RAAFAT.SOLIMAN@shell.com</t>
+  </si>
+  <si>
+    <t>IPSec_Gateway_Raafat-FW</t>
+  </si>
+  <si>
+    <t>IPSec_Tunnel_Raafat-FW</t>
+  </si>
+  <si>
+    <t>tunnel.11</t>
+  </si>
+  <si>
+    <t>213.46.228.196</t>
+  </si>
+  <si>
+    <t>Peer_Type</t>
+  </si>
+  <si>
+    <t>local_id</t>
+  </si>
+  <si>
+    <t>Local_Type</t>
+  </si>
+  <si>
+    <t>ipaddr</t>
+  </si>
+  <si>
+    <t>ufqdn</t>
+  </si>
+  <si>
+    <t>192.168.178.156/24</t>
+  </si>
+  <si>
+    <t>uqfdn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IP </t>
+  </si>
+  <si>
+    <t>IPSec_Tunnel_Test_Tenant</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -542,6 +602,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -840,7 +908,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -883,8 +951,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -892,8 +961,11 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -927,6 +999,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1267,16 +1340,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07EFEA9B-6B0F-49FF-A3F2-CCAD28442207}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:O102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
-      <selection activeCell="B81" sqref="B81"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36.7265625" customWidth="1"/>
-    <col min="2" max="2" width="52" style="1" customWidth="1"/>
+    <col min="2" max="2" width="62" style="1" customWidth="1"/>
+    <col min="14" max="14" width="31.90625" customWidth="1"/>
+    <col min="15" max="15" width="28.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
@@ -1300,599 +1375,744 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>15</v>
+        <v>108</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>111</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>26</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>110</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>28</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>109</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>32</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>49</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>51</v>
+        <v>114</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>13</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>115</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>116</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>53</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>117</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>56</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>57</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>58</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>59</v>
+        <v>118</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>58</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>63</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>64</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>9</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>122</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>66</v>
+        <v>6</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
-        <v>71</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>73</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>75</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+      <c r="N49" t="s">
+        <v>138</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="N50" t="s">
+        <v>42</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
+        <v>138</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="N51" t="s">
+        <v>137</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>81</v>
-      </c>
-      <c r="B52" s="1">
-        <v>65103</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
+        <v>42</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="O52" s="3"/>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>82</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>86</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
+        <v>137</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="O53" s="3"/>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B54" s="3"/>
+      <c r="N54" t="s">
+        <v>136</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B55" s="3"/>
+      <c r="N55" t="s">
+        <v>43</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>88</v>
+        <v>136</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+      <c r="N56" t="s">
+        <v>44</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>90</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N57" t="s">
+        <v>45</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>91</v>
-      </c>
-      <c r="B58" s="2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.35">
+        <v>44</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="N58" t="s">
+        <v>101</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.35">
+        <v>133</v>
+      </c>
+      <c r="O59" s="1"/>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>94</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>95</v>
+        <v>46</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>96</v>
+        <v>47</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.35">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>49</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>99</v>
-      </c>
-      <c r="B65" s="1">
-        <v>65101</v>
+        <v>51</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>100</v>
-      </c>
-      <c r="B66" s="1">
-        <v>65101</v>
+        <v>53</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>101</v>
+        <v>56</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>102</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>103</v>
+        <v>58</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>104</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>105</v>
+        <v>60</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
-        <v>106</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>108</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>109</v>
+        <v>62</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>110</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>102</v>
+        <v>63</v>
+      </c>
+      <c r="B73" s="1">
+        <v>65103</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>111</v>
+        <v>64</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>104</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>112</v>
+        <v>66</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>113</v>
+        <v>67</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>114</v>
+        <v>68</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>115</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>116</v>
+        <v>70</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>117</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>115</v>
+        <v>72</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>118</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>109</v>
+        <v>73</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>119</v>
+        <v>74</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>102</v>
+        <v>16</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>124</v>
+        <v>75</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>104</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>76</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" t="s">
+        <v>77</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>78</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>81</v>
+      </c>
+      <c r="B86" s="1">
+        <v>65101</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="1">
+        <v>65101</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>83</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>85</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>87</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>88</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>89</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" t="s">
+        <v>91</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" t="s">
+        <v>92</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" t="s">
+        <v>95</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" t="s">
+        <v>99</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B53" r:id="rId1" display="RAAFAT.SOLIMAN@shell.com" xr:uid="{E2B1982A-F6CF-4C60-ABE5-05FEAD6DC577}"/>
+    <hyperlink ref="B57" r:id="rId2" xr:uid="{6889103B-82E6-4D82-9906-95D94A064F5D}"/>
+    <hyperlink ref="O51" r:id="rId3" xr:uid="{8F1275F1-8E51-45C5-8846-43A5AF4D74EE}"/>
+    <hyperlink ref="B58" r:id="rId4" xr:uid="{7DE5286F-1609-4056-91F4-116A4C37F23B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
   <ignoredErrors>
-    <ignoredError sqref="B51 B57:B58" numberStoredAsText="1"/>
+    <ignoredError sqref="B72 B78:B79" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>